<commit_message>
feat: update draft exploration
</commit_message>
<xml_diff>
--- a/data/raw-data/traits/GIFT_metadata_filled.xlsx
+++ b/data/raw-data/traits/GIFT_metadata_filled.xlsx
@@ -1304,7 +1304,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A66" zoomScale="140" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="140" workbookViewId="0">
       <selection activeCell="K24" activeCellId="0" sqref="K24"/>
     </sheetView>
   </sheetViews>
@@ -1345,7 +1345,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" hidden="1">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" hidden="1">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" hidden="1">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" hidden="1">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" hidden="1">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" hidden="1">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" hidden="1">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" hidden="1">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" hidden="1">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" hidden="1">
       <c r="A15">
         <v>6</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" hidden="1">
       <c r="A16">
         <v>6</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" hidden="1">
       <c r="A17">
         <v>6</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" hidden="1">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" hidden="1">
       <c r="A26">
         <v>3</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" hidden="1">
       <c r="A27">
         <v>6</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" hidden="1">
       <c r="A31">
         <v>3</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" hidden="1">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" hidden="1">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" hidden="1">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" hidden="1">
       <c r="A35">
         <v>2</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" hidden="1">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" hidden="1">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" hidden="1">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" hidden="1">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" hidden="1">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" hidden="1">
       <c r="A48">
         <v>1</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" hidden="1">
       <c r="A49">
         <v>3</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" hidden="1">
       <c r="A50">
         <v>3</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" hidden="1">
       <c r="A51">
         <v>4</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" ht="285">
+    <row r="52" ht="285" hidden="1">
       <c r="A52">
         <v>3</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" hidden="1">
       <c r="A53">
         <v>3</v>
       </c>
@@ -3159,7 +3159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" hidden="1">
       <c r="A54">
         <v>3</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" hidden="1">
       <c r="A55">
         <v>3</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" hidden="1">
       <c r="A56">
         <v>3</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" hidden="1">
       <c r="A57">
         <v>6</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" hidden="1">
       <c r="A59">
         <v>3</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" hidden="1">
       <c r="A60">
         <v>3</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" hidden="1">
       <c r="A61">
         <v>4</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" ht="272">
+    <row r="63" ht="272" hidden="1">
       <c r="A63">
         <v>4</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>2304</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" hidden="1">
       <c r="A64">
         <v>1</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" hidden="1">
       <c r="A67">
         <v>1</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" hidden="1">
       <c r="A68">
         <v>3</v>
       </c>
@@ -3742,7 +3742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" hidden="1">
       <c r="A71">
         <v>4</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" hidden="1">
       <c r="A73">
         <v>4</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" hidden="1">
       <c r="A74">
         <v>4</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" hidden="1">
       <c r="A75">
         <v>3</v>
       </c>
@@ -3917,7 +3917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" hidden="1">
       <c r="A76">
         <v>3</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" hidden="1">
       <c r="A77">
         <v>5</v>
       </c>
@@ -3987,7 +3987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" hidden="1">
       <c r="A78">
         <v>3</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" hidden="1">
       <c r="A79">
         <v>4</v>
       </c>
@@ -4057,7 +4057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" hidden="1">
       <c r="A80">
         <v>4</v>
       </c>
@@ -4124,7 +4124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" hidden="1">
       <c r="A82">
         <v>3</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" hidden="1">
       <c r="A83">
         <v>3</v>
       </c>
@@ -4194,7 +4194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" hidden="1">
       <c r="A84">
         <v>4</v>
       </c>
@@ -4229,7 +4229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" hidden="1">
       <c r="A85">
         <v>4</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" hidden="1">
       <c r="A86">
         <v>3</v>
       </c>
@@ -4299,7 +4299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" hidden="1">
       <c r="A87">
         <v>4</v>
       </c>
@@ -4334,7 +4334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" hidden="1">
       <c r="A88">
         <v>4</v>
       </c>
@@ -4369,7 +4369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" hidden="1">
       <c r="A89">
         <v>4</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" hidden="1">
       <c r="A90">
         <v>4</v>
       </c>
@@ -4474,7 +4474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" hidden="1">
       <c r="A92">
         <v>5</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" hidden="1">
       <c r="A93">
         <v>4</v>
       </c>
@@ -4544,7 +4544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" hidden="1">
       <c r="A94">
         <v>4</v>
       </c>
@@ -4614,7 +4614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" hidden="1">
       <c r="A96">
         <v>6</v>
       </c>
@@ -4649,7 +4649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" hidden="1">
       <c r="A97">
         <v>6</v>
       </c>
@@ -4684,7 +4684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" hidden="1">
       <c r="A98">
         <v>3</v>
       </c>
@@ -4719,7 +4719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" hidden="1">
       <c r="A99">
         <v>4</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" hidden="1">
       <c r="A100">
         <v>1</v>
       </c>
@@ -4789,7 +4789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" hidden="1">
       <c r="A101">
         <v>3</v>
       </c>
@@ -4824,7 +4824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" hidden="1">
       <c r="A102">
         <v>2</v>
       </c>
@@ -4859,7 +4859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" hidden="1">
       <c r="A103">
         <v>3</v>
       </c>
@@ -4894,7 +4894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" hidden="1">
       <c r="A104">
         <v>3</v>
       </c>
@@ -4929,7 +4929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" hidden="1">
       <c r="A105">
         <v>3</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" hidden="1">
       <c r="A106">
         <v>4</v>
       </c>
@@ -4999,7 +4999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" hidden="1">
       <c r="A107">
         <v>4</v>
       </c>
@@ -5034,7 +5034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" hidden="1">
       <c r="A108">
         <v>3</v>
       </c>
@@ -5069,7 +5069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" hidden="1">
       <c r="A109">
         <v>3</v>
       </c>
@@ -5104,7 +5104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" hidden="1">
       <c r="A110">
         <v>1</v>
       </c>
@@ -5141,6 +5141,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K110">
+    <filterColumn colId="10">
+      <filters>
+        <filter val="TRUE"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A2:K110">
       <sortCondition descending="1" ref="J1:J110"/>
     </sortState>

</xml_diff>